<commit_message>
Update data files and scripts
- Updated Disruption Index data
- Daily brief dashboard updates
- Parabolic backtest improvements
- Added parabolic optimizer script

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Disruption Index.xlsx
+++ b/Disruption Index.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29725"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daqui\PycharmProjects\PythonProject1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7B8498-C055-4187-858D-481F736FB521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287711D6-8548-488A-A68A-787FDC335DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5690" yWindow="2420" windowWidth="16800" windowHeight="9680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-2865" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="353">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -1062,12 +1062,45 @@
   </si>
   <si>
     <t>TE</t>
+  </si>
+  <si>
+    <t>tsem</t>
+  </si>
+  <si>
+    <t>enr</t>
+  </si>
+  <si>
+    <t>bwtx</t>
+  </si>
+  <si>
+    <t>sym</t>
+  </si>
+  <si>
+    <t>alb</t>
+  </si>
+  <si>
+    <t>cifr</t>
+  </si>
+  <si>
+    <t>clsk</t>
+  </si>
+  <si>
+    <t>wulf</t>
+  </si>
+  <si>
+    <t>iren</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> app</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="000000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1118,16 +1151,67 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1436,10 +1520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C341"/>
+  <dimension ref="A1:C354"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A331" workbookViewId="0">
+      <selection activeCell="L346" sqref="L345:L346"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4164,9 +4248,78 @@
         <v>341</v>
       </c>
     </row>
+    <row r="342" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B342" s="2">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="343" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B343">
+        <v>6857</v>
+      </c>
+    </row>
+    <row r="344" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B344" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="345" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B345" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="346" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B346">
+        <v>2383</v>
+      </c>
+    </row>
+    <row r="347" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B347" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="348" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B348" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="349" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B349" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="350" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B350" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="351" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B351" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="352" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B352" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="353" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B353" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="354" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B354" t="s">
+        <v>352</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B342">
+    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>